<commit_message>
made teh foreign key indexed
</commit_message>
<xml_diff>
--- a/Oracle/OracleStat.xlsx
+++ b/Oracle/OracleStat.xlsx
@@ -451,7 +451,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -475,7 +475,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -499,7 +499,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -507,7 +507,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -515,7 +515,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -523,7 +523,7 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -531,7 +531,7 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -539,7 +539,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -547,7 +547,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>54</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -555,7 +555,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -563,7 +563,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -571,7 +571,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -579,7 +579,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -587,7 +587,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>63</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -595,7 +595,7 @@
         <v>20</v>
       </c>
       <c r="C20">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -603,7 +603,7 @@
         <v>21</v>
       </c>
       <c r="C21">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -611,7 +611,7 @@
         <v>22</v>
       </c>
       <c r="C22">
-        <v>250</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -619,7 +619,7 @@
         <v>23</v>
       </c>
       <c r="C23">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -627,7 +627,7 @@
         <v>24</v>
       </c>
       <c r="C24">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -635,7 +635,7 @@
         <v>25</v>
       </c>
       <c r="C25">
-        <v>1242</v>
+        <v>940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>